<commit_message>
Updated Risk Management log
</commit_message>
<xml_diff>
--- a/Documentation/8.0 Risk Assessment/Risk Management Log v2.4.xlsx
+++ b/Documentation/8.0 Risk Assessment/Risk Management Log v2.4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
   <si>
     <t xml:space="preserve">Risk ID </t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>Stephen to implement over christmas</t>
+  </si>
+  <si>
+    <t>API Security is such that anyone that can authenticate with the application is able to make any requests change anything on the application.</t>
+  </si>
+  <si>
+    <t>Implement methods to check who they are and what they are trying to change</t>
   </si>
 </sst>
 </file>
@@ -826,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -918,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" ref="H4:H24" si="0">F4*G4</f>
+        <f t="shared" ref="H4:H25" si="0">F4*G4</f>
         <v>10</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -941,7 +947,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="str">
-        <f t="shared" ref="C5:C24" si="1">IF(H5&lt;=7, "Low Risk",IF(H5&gt;=17,"High Risk","Medium Risk"))</f>
+        <f t="shared" ref="C5:C25" si="1">IF(H5&lt;=7, "Low Risk",IF(H5&gt;=17,"High Risk","Medium Risk"))</f>
         <v>Low Risk</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1762,16 +1768,38 @@
       <c r="B25" s="8">
         <v>22</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="7"/>
+      <c r="C25" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>High Risk</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="5">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5">
+        <v>5</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L25" s="7">
+        <v>42057</v>
+      </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
     </row>

</xml_diff>